<commit_message>
Results for IK-IP and Modulo Metric
</commit_message>
<xml_diff>
--- a/results-normalized/Normalized.xlsx
+++ b/results-normalized/Normalized.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf2ea51ea12e088c/Documents/CMU/22Spring/16711/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf2ea51ea12e088c/Documents/CMU/22Spring/16711/Project/results-normalized/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{2A0944E2-ED36-4A28-9223-0874B57D5ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C73FE111-3DB3-489C-9886-2CB564629D06}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{2A0944E2-ED36-4A28-9223-0874B57D5ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74D0FF90-36CE-4E35-92CB-B3446F9941D8}"/>
   <bookViews>
-    <workbookView xWindow="28718" yWindow="-3720" windowWidth="16364" windowHeight="14123" xr2:uid="{6767D876-5173-4B97-963C-A9C26995BB88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14565" windowHeight="15563" xr2:uid="{6767D876-5173-4B97-963C-A9C26995BB88}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="2" r:id="rId1"/>
@@ -191,6 +191,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,14 +223,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -277,12 +287,12 @@
     <sortCondition ref="D2:D28"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{92F7EE35-878D-4070-AA11-F3C07002DEA9}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{512C8484-5DEB-42FE-BF64-81B0A7CB4699}" uniqueName="2" name="Column1" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{AF465138-65C6-4F8B-981F-88E2404AEFD0}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{CA35BECE-4F5F-42AF-A1E1-23A21BA02A99}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{72A86B42-18BE-4857-97E5-0996A742CF1F}" uniqueName="5" name="Column4" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{D9320416-1783-441F-B016-09F9CCA3414A}" uniqueName="6" name="Column5" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{92F7EE35-878D-4070-AA11-F3C07002DEA9}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{512C8484-5DEB-42FE-BF64-81B0A7CB4699}" uniqueName="2" name="Column1" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{AF465138-65C6-4F8B-981F-88E2404AEFD0}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{CA35BECE-4F5F-42AF-A1E1-23A21BA02A99}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{72A86B42-18BE-4857-97E5-0996A742CF1F}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D9320416-1783-441F-B016-09F9CCA3414A}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -588,7 +598,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -631,10 +641,10 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>1.1982999999999999</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>0.2074</v>
       </c>
     </row>
@@ -651,10 +661,10 @@
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>2.0318000000000001</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.33</v>
       </c>
     </row>
@@ -671,10 +681,10 @@
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>2.2227000000000001</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.54779999999999995</v>
       </c>
     </row>
@@ -691,10 +701,10 @@
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>1.0544</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>3.5200000000000002E-2</v>
       </c>
     </row>
@@ -711,10 +721,10 @@
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>1.1809000000000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>0.1069</v>
       </c>
     </row>
@@ -731,10 +741,10 @@
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1.0347999999999999</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
@@ -751,10 +761,10 @@
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>1.1882999999999999</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -771,10 +781,10 @@
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>28.190899999999999</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>22.679300000000001</v>
       </c>
     </row>
@@ -791,10 +801,10 @@
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1.5682</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>0.85</v>
       </c>
     </row>
@@ -811,10 +821,10 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>3.3195999999999999</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>0.13139999999999999</v>
       </c>
     </row>
@@ -831,10 +841,10 @@
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>3.4300999999999999</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>0.48959999999999998</v>
       </c>
     </row>
@@ -851,10 +861,10 @@
       <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>2.9466000000000001</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>0.52729999999999999</v>
       </c>
     </row>
@@ -871,10 +881,10 @@
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>1.0322</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
@@ -891,10 +901,10 @@
       <c r="D15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>10.3665</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>6.4158999999999997</v>
       </c>
     </row>
@@ -911,10 +921,10 @@
       <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>3.9214000000000002</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>1.931</v>
       </c>
     </row>
@@ -931,10 +941,10 @@
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>5.2460000000000004</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>3.1242999999999999</v>
       </c>
     </row>
@@ -951,10 +961,10 @@
       <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>123.4081</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>26.523900000000001</v>
       </c>
     </row>
@@ -971,10 +981,10 @@
       <c r="D19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>4.0076999999999998</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>2.6015000000000001</v>
       </c>
     </row>
@@ -991,10 +1001,10 @@
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>1.1207</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>0.1779</v>
       </c>
     </row>
@@ -1011,10 +1021,10 @@
       <c r="D21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>3.3736000000000002</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>0.32640000000000002</v>
       </c>
     </row>
@@ -1031,10 +1041,10 @@
       <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>2.5503999999999998</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>0.50019999999999998</v>
       </c>
     </row>
@@ -1051,10 +1061,10 @@
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>55.648299999999999</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>9.7886000000000006</v>
       </c>
     </row>
@@ -1071,10 +1081,10 @@
       <c r="D24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>25.311</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>16.2379</v>
       </c>
     </row>
@@ -1091,10 +1101,10 @@
       <c r="D25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>148.4838</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>125.1532</v>
       </c>
     </row>
@@ -1111,10 +1121,10 @@
       <c r="D26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>114.6358</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1131,10 +1141,10 @@
       <c r="D27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>116.9019</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>53.087800000000001</v>
       </c>
     </row>
@@ -1151,10 +1161,10 @@
       <c r="D28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>849.476</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>216.36070000000001</v>
       </c>
     </row>

</xml_diff>